<commit_message>
Adding full vaccination prediction, notebook daily cases prediction with full vaccination And FB mobility
</commit_message>
<xml_diff>
--- a/dataset/kawaldata_clean.xlsx
+++ b/dataset/kawaldata_clean.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR565"/>
+  <dimension ref="A1:AR568"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -59474,145 +59474,379 @@
       <c r="A537" s="1" t="n">
         <v>535</v>
       </c>
-      <c r="B537" t="inlineStr"/>
-      <c r="C537" t="inlineStr"/>
-      <c r="D537" t="inlineStr"/>
-      <c r="E537" t="inlineStr"/>
-      <c r="F537" t="inlineStr"/>
-      <c r="G537" t="inlineStr"/>
-      <c r="H537" t="inlineStr"/>
-      <c r="I537" t="inlineStr"/>
-      <c r="J537" t="inlineStr"/>
-      <c r="K537" t="inlineStr"/>
-      <c r="L537" t="inlineStr"/>
-      <c r="M537" t="inlineStr"/>
-      <c r="N537" t="inlineStr"/>
+      <c r="B537" s="2" t="n">
+        <v>44428</v>
+      </c>
+      <c r="C537" t="n">
+        <v>20004</v>
+      </c>
+      <c r="D537" t="n">
+        <v>3950304</v>
+      </c>
+      <c r="E537" t="n">
+        <v>327286</v>
+      </c>
+      <c r="F537" t="n">
+        <v>26122</v>
+      </c>
+      <c r="G537" t="n">
+        <v>3499037</v>
+      </c>
+      <c r="H537" t="n">
+        <v>1348</v>
+      </c>
+      <c r="I537" t="n">
+        <v>123981</v>
+      </c>
+      <c r="J537" t="n">
+        <v>0.03138517947</v>
+      </c>
+      <c r="K537" t="n">
+        <v>0.03422036545</v>
+      </c>
+      <c r="L537" t="n">
+        <v>30213170</v>
+      </c>
+      <c r="M537" t="n">
+        <v>20299651</v>
+      </c>
+      <c r="N537" t="n">
+        <v>16349347</v>
+      </c>
       <c r="O537" t="inlineStr"/>
       <c r="P537" t="inlineStr"/>
-      <c r="Q537" t="inlineStr"/>
-      <c r="R537" t="inlineStr"/>
-      <c r="S537" t="inlineStr"/>
-      <c r="T537" t="inlineStr"/>
-      <c r="U537" t="inlineStr"/>
-      <c r="V537" t="inlineStr"/>
+      <c r="Q537" t="n">
+        <v>202484</v>
+      </c>
+      <c r="R537" t="n">
+        <v>101685</v>
+      </c>
+      <c r="S537" t="n">
+        <v>100799</v>
+      </c>
+      <c r="T537" t="n">
+        <v>113847</v>
+      </c>
+      <c r="U537" t="n">
+        <v>38095</v>
+      </c>
+      <c r="V537" t="n">
+        <v>75752</v>
+      </c>
       <c r="W537" t="inlineStr"/>
-      <c r="X537" t="inlineStr"/>
-      <c r="Y537" t="inlineStr"/>
-      <c r="Z537" t="inlineStr"/>
-      <c r="AA537" t="inlineStr"/>
-      <c r="AB537" t="inlineStr"/>
-      <c r="AC537" t="inlineStr"/>
-      <c r="AD537" t="inlineStr"/>
-      <c r="AE537" t="inlineStr"/>
-      <c r="AF537" t="inlineStr"/>
-      <c r="AG537" t="inlineStr"/>
-      <c r="AH537" t="inlineStr"/>
+      <c r="X537" t="n">
+        <v>75183.89259</v>
+      </c>
+      <c r="Y537" t="n">
+        <v>7.648315168</v>
+      </c>
+      <c r="Z537" t="n">
+        <v>5.138756663</v>
+      </c>
+      <c r="AA537" t="n">
+        <v>5.691211758</v>
+      </c>
+      <c r="AB537" t="n">
+        <v>0.1945996017</v>
+      </c>
+      <c r="AC537" t="n">
+        <v>0.1757095049</v>
+      </c>
+      <c r="AD537" t="n">
+        <v>0.00508968781</v>
+      </c>
+      <c r="AE537" t="n">
+        <v>0.2066054738</v>
+      </c>
+      <c r="AF537" t="n">
+        <v>178151.7143</v>
+      </c>
+      <c r="AG537" t="n">
+        <v>100509.7143</v>
+      </c>
+      <c r="AH537" t="n">
+        <v>1.772482546</v>
+      </c>
       <c r="AI537" t="inlineStr"/>
-      <c r="AJ537" t="inlineStr"/>
-      <c r="AK537" t="inlineStr"/>
-      <c r="AL537" t="inlineStr"/>
-      <c r="AM537" t="inlineStr"/>
-      <c r="AN537" t="inlineStr"/>
-      <c r="AO537" t="inlineStr"/>
-      <c r="AP537" t="inlineStr"/>
-      <c r="AQ537" t="inlineStr"/>
-      <c r="AR537" t="inlineStr"/>
+      <c r="AJ537" t="n">
+        <v>55995182</v>
+      </c>
+      <c r="AK537" t="n">
+        <v>30585478</v>
+      </c>
+      <c r="AL537" t="n">
+        <v>365335</v>
+      </c>
+      <c r="AM537" t="n">
+        <v>0.207389563</v>
+      </c>
+      <c r="AN537" t="n">
+        <v>0.1132795481</v>
+      </c>
+      <c r="AO537" t="n">
+        <v>357948</v>
+      </c>
+      <c r="AP537" t="n">
+        <v>355245</v>
+      </c>
+      <c r="AQ537" t="n">
+        <v>749021</v>
+      </c>
+      <c r="AR537" t="n">
+        <v>464801.5714</v>
+      </c>
     </row>
     <row r="538">
       <c r="A538" s="1" t="n">
         <v>536</v>
       </c>
-      <c r="B538" t="inlineStr"/>
-      <c r="C538" t="inlineStr"/>
-      <c r="D538" t="inlineStr"/>
-      <c r="E538" t="inlineStr"/>
-      <c r="F538" t="inlineStr"/>
-      <c r="G538" t="inlineStr"/>
-      <c r="H538" t="inlineStr"/>
-      <c r="I538" t="inlineStr"/>
-      <c r="J538" t="inlineStr"/>
-      <c r="K538" t="inlineStr"/>
-      <c r="L538" t="inlineStr"/>
-      <c r="M538" t="inlineStr"/>
-      <c r="N538" t="inlineStr"/>
+      <c r="B538" s="2" t="n">
+        <v>44429</v>
+      </c>
+      <c r="C538" t="n">
+        <v>16744</v>
+      </c>
+      <c r="D538" t="n">
+        <v>3967048</v>
+      </c>
+      <c r="E538" t="n">
+        <v>319658</v>
+      </c>
+      <c r="F538" t="n">
+        <v>23011</v>
+      </c>
+      <c r="G538" t="n">
+        <v>3522048</v>
+      </c>
+      <c r="H538" t="n">
+        <v>1361</v>
+      </c>
+      <c r="I538" t="n">
+        <v>125342</v>
+      </c>
+      <c r="J538" t="n">
+        <v>0.03159578609</v>
+      </c>
+      <c r="K538" t="n">
+        <v>0.03436484719</v>
+      </c>
+      <c r="L538" t="n">
+        <v>30413420</v>
+      </c>
+      <c r="M538" t="n">
+        <v>20415957</v>
+      </c>
+      <c r="N538" t="n">
+        <v>16448909</v>
+      </c>
       <c r="O538" t="inlineStr"/>
       <c r="P538" t="inlineStr"/>
-      <c r="Q538" t="inlineStr"/>
-      <c r="R538" t="inlineStr"/>
-      <c r="S538" t="inlineStr"/>
-      <c r="T538" t="inlineStr"/>
-      <c r="U538" t="inlineStr"/>
-      <c r="V538" t="inlineStr"/>
+      <c r="Q538" t="n">
+        <v>200250</v>
+      </c>
+      <c r="R538" t="n">
+        <v>94985</v>
+      </c>
+      <c r="S538" t="n">
+        <v>105265</v>
+      </c>
+      <c r="T538" t="n">
+        <v>116306</v>
+      </c>
+      <c r="U538" t="n">
+        <v>37275</v>
+      </c>
+      <c r="V538" t="n">
+        <v>79031</v>
+      </c>
       <c r="W538" t="inlineStr"/>
-      <c r="X538" t="inlineStr"/>
-      <c r="Y538" t="inlineStr"/>
-      <c r="Z538" t="inlineStr"/>
-      <c r="AA538" t="inlineStr"/>
-      <c r="AB538" t="inlineStr"/>
-      <c r="AC538" t="inlineStr"/>
-      <c r="AD538" t="inlineStr"/>
-      <c r="AE538" t="inlineStr"/>
-      <c r="AF538" t="inlineStr"/>
-      <c r="AG538" t="inlineStr"/>
-      <c r="AH538" t="inlineStr"/>
+      <c r="X538" t="n">
+        <v>75614.65556</v>
+      </c>
+      <c r="Y538" t="n">
+        <v>7.666511724</v>
+      </c>
+      <c r="Z538" t="n">
+        <v>5.146385171</v>
+      </c>
+      <c r="AA538" t="n">
+        <v>6.946129957</v>
+      </c>
+      <c r="AB538" t="n">
+        <v>0.1943111459</v>
+      </c>
+      <c r="AC538" t="n">
+        <v>0.1439650577</v>
+      </c>
+      <c r="AD538" t="n">
+        <v>0.004238661126</v>
+      </c>
+      <c r="AE538" t="n">
+        <v>0.1925235559</v>
+      </c>
+      <c r="AF538" t="n">
+        <v>174961.4286</v>
+      </c>
+      <c r="AG538" t="n">
+        <v>99065.42857</v>
+      </c>
+      <c r="AH538" t="n">
+        <v>1.766119938</v>
+      </c>
       <c r="AI538" t="inlineStr"/>
-      <c r="AJ538" t="inlineStr"/>
-      <c r="AK538" t="inlineStr"/>
-      <c r="AL538" t="inlineStr"/>
-      <c r="AM538" t="inlineStr"/>
-      <c r="AN538" t="inlineStr"/>
-      <c r="AO538" t="inlineStr"/>
-      <c r="AP538" t="inlineStr"/>
-      <c r="AQ538" t="inlineStr"/>
-      <c r="AR538" t="inlineStr"/>
+      <c r="AJ538" t="n">
+        <v>57282879</v>
+      </c>
+      <c r="AK538" t="n">
+        <v>31566685</v>
+      </c>
+      <c r="AL538" t="n">
+        <v>423627</v>
+      </c>
+      <c r="AM538" t="n">
+        <v>0.2121588111</v>
+      </c>
+      <c r="AN538" t="n">
+        <v>0.1169136481</v>
+      </c>
+      <c r="AO538" t="n">
+        <v>598148</v>
+      </c>
+      <c r="AP538" t="n">
+        <v>619482</v>
+      </c>
+      <c r="AQ538" t="n">
+        <v>1275922</v>
+      </c>
+      <c r="AR538" t="n">
+        <v>461055.5714</v>
+      </c>
     </row>
     <row r="539">
       <c r="A539" s="1" t="n">
         <v>537</v>
       </c>
-      <c r="B539" t="inlineStr"/>
-      <c r="C539" t="inlineStr"/>
-      <c r="D539" t="inlineStr"/>
-      <c r="E539" t="inlineStr"/>
-      <c r="F539" t="inlineStr"/>
-      <c r="G539" t="inlineStr"/>
-      <c r="H539" t="inlineStr"/>
-      <c r="I539" t="inlineStr"/>
-      <c r="J539" t="inlineStr"/>
-      <c r="K539" t="inlineStr"/>
-      <c r="L539" t="inlineStr"/>
-      <c r="M539" t="inlineStr"/>
-      <c r="N539" t="inlineStr"/>
+      <c r="B539" s="2" t="n">
+        <v>44430</v>
+      </c>
+      <c r="C539" t="n">
+        <v>12408</v>
+      </c>
+      <c r="D539" t="n">
+        <v>3979456</v>
+      </c>
+      <c r="E539" t="n">
+        <v>306760</v>
+      </c>
+      <c r="F539" t="n">
+        <v>24276</v>
+      </c>
+      <c r="G539" t="n">
+        <v>3546324</v>
+      </c>
+      <c r="H539" t="n">
+        <v>1030</v>
+      </c>
+      <c r="I539" t="n">
+        <v>126372</v>
+      </c>
+      <c r="J539" t="n">
+        <v>0.03175609933</v>
+      </c>
+      <c r="K539" t="n">
+        <v>0.03440851081</v>
+      </c>
+      <c r="L539" t="n">
+        <v>30561830</v>
+      </c>
+      <c r="M539" t="n">
+        <v>20501173</v>
+      </c>
+      <c r="N539" t="n">
+        <v>16521717</v>
+      </c>
       <c r="O539" t="inlineStr"/>
       <c r="P539" t="inlineStr"/>
-      <c r="Q539" t="inlineStr"/>
-      <c r="R539" t="inlineStr"/>
-      <c r="S539" t="inlineStr"/>
-      <c r="T539" t="inlineStr"/>
-      <c r="U539" t="inlineStr"/>
-      <c r="V539" t="inlineStr"/>
+      <c r="Q539" t="n">
+        <v>148410</v>
+      </c>
+      <c r="R539" t="n">
+        <v>76742</v>
+      </c>
+      <c r="S539" t="n">
+        <v>71668</v>
+      </c>
+      <c r="T539" t="n">
+        <v>85216</v>
+      </c>
+      <c r="U539" t="n">
+        <v>31691</v>
+      </c>
+      <c r="V539" t="n">
+        <v>53525</v>
+      </c>
       <c r="W539" t="inlineStr"/>
-      <c r="X539" t="inlineStr"/>
-      <c r="Y539" t="inlineStr"/>
-      <c r="Z539" t="inlineStr"/>
-      <c r="AA539" t="inlineStr"/>
-      <c r="AB539" t="inlineStr"/>
-      <c r="AC539" t="inlineStr"/>
-      <c r="AD539" t="inlineStr"/>
-      <c r="AE539" t="inlineStr"/>
-      <c r="AF539" t="inlineStr"/>
-      <c r="AG539" t="inlineStr"/>
-      <c r="AH539" t="inlineStr"/>
+      <c r="X539" t="n">
+        <v>75930.27037</v>
+      </c>
+      <c r="Y539" t="n">
+        <v>7.679901474</v>
+      </c>
+      <c r="Z539" t="n">
+        <v>5.151752652</v>
+      </c>
+      <c r="AA539" t="n">
+        <v>6.867827208</v>
+      </c>
+      <c r="AB539" t="n">
+        <v>0.1941086981</v>
+      </c>
+      <c r="AC539" t="n">
+        <v>0.1456064589</v>
+      </c>
+      <c r="AD539" t="n">
+        <v>0.003127766541</v>
+      </c>
+      <c r="AE539" t="n">
+        <v>0.1815951668</v>
+      </c>
+      <c r="AF539" t="n">
+        <v>173423.1429</v>
+      </c>
+      <c r="AG539" t="n">
+        <v>98415.14286000001</v>
+      </c>
+      <c r="AH539" t="n">
+        <v>1.762159133</v>
+      </c>
       <c r="AI539" t="inlineStr"/>
-      <c r="AJ539" t="inlineStr"/>
-      <c r="AK539" t="inlineStr"/>
-      <c r="AL539" t="inlineStr"/>
-      <c r="AM539" t="inlineStr"/>
-      <c r="AN539" t="inlineStr"/>
-      <c r="AO539" t="inlineStr"/>
-      <c r="AP539" t="inlineStr"/>
-      <c r="AQ539" t="inlineStr"/>
-      <c r="AR539" t="inlineStr"/>
+      <c r="AJ539" t="n">
+        <v>57338901</v>
+      </c>
+      <c r="AK539" t="n">
+        <v>31601400</v>
+      </c>
+      <c r="AL539" t="n">
+        <v>424625</v>
+      </c>
+      <c r="AM539" t="n">
+        <v>0.2123663</v>
+      </c>
+      <c r="AN539" t="n">
+        <v>0.1170422222</v>
+      </c>
+      <c r="AO539" t="n">
+        <v>56022</v>
+      </c>
+      <c r="AP539" t="n">
+        <v>34715</v>
+      </c>
+      <c r="AQ539" t="n">
+        <v>91735</v>
+      </c>
+      <c r="AR539" t="n">
+        <v>423032.8571</v>
+      </c>
     </row>
     <row r="540">
       <c r="A540" s="1" t="n">
@@ -60862,6 +61096,150 @@
       <c r="AQ565" t="inlineStr"/>
       <c r="AR565" t="inlineStr"/>
     </row>
+    <row r="566">
+      <c r="A566" s="1" t="n">
+        <v>564</v>
+      </c>
+      <c r="B566" t="inlineStr"/>
+      <c r="C566" t="inlineStr"/>
+      <c r="D566" t="inlineStr"/>
+      <c r="E566" t="inlineStr"/>
+      <c r="F566" t="inlineStr"/>
+      <c r="G566" t="inlineStr"/>
+      <c r="H566" t="inlineStr"/>
+      <c r="I566" t="inlineStr"/>
+      <c r="J566" t="inlineStr"/>
+      <c r="K566" t="inlineStr"/>
+      <c r="L566" t="inlineStr"/>
+      <c r="M566" t="inlineStr"/>
+      <c r="N566" t="inlineStr"/>
+      <c r="O566" t="inlineStr"/>
+      <c r="P566" t="inlineStr"/>
+      <c r="Q566" t="inlineStr"/>
+      <c r="R566" t="inlineStr"/>
+      <c r="S566" t="inlineStr"/>
+      <c r="T566" t="inlineStr"/>
+      <c r="U566" t="inlineStr"/>
+      <c r="V566" t="inlineStr"/>
+      <c r="W566" t="inlineStr"/>
+      <c r="X566" t="inlineStr"/>
+      <c r="Y566" t="inlineStr"/>
+      <c r="Z566" t="inlineStr"/>
+      <c r="AA566" t="inlineStr"/>
+      <c r="AB566" t="inlineStr"/>
+      <c r="AC566" t="inlineStr"/>
+      <c r="AD566" t="inlineStr"/>
+      <c r="AE566" t="inlineStr"/>
+      <c r="AF566" t="inlineStr"/>
+      <c r="AG566" t="inlineStr"/>
+      <c r="AH566" t="inlineStr"/>
+      <c r="AI566" t="inlineStr"/>
+      <c r="AJ566" t="inlineStr"/>
+      <c r="AK566" t="inlineStr"/>
+      <c r="AL566" t="inlineStr"/>
+      <c r="AM566" t="inlineStr"/>
+      <c r="AN566" t="inlineStr"/>
+      <c r="AO566" t="inlineStr"/>
+      <c r="AP566" t="inlineStr"/>
+      <c r="AQ566" t="inlineStr"/>
+      <c r="AR566" t="inlineStr"/>
+    </row>
+    <row r="567">
+      <c r="A567" s="1" t="n">
+        <v>565</v>
+      </c>
+      <c r="B567" t="inlineStr"/>
+      <c r="C567" t="inlineStr"/>
+      <c r="D567" t="inlineStr"/>
+      <c r="E567" t="inlineStr"/>
+      <c r="F567" t="inlineStr"/>
+      <c r="G567" t="inlineStr"/>
+      <c r="H567" t="inlineStr"/>
+      <c r="I567" t="inlineStr"/>
+      <c r="J567" t="inlineStr"/>
+      <c r="K567" t="inlineStr"/>
+      <c r="L567" t="inlineStr"/>
+      <c r="M567" t="inlineStr"/>
+      <c r="N567" t="inlineStr"/>
+      <c r="O567" t="inlineStr"/>
+      <c r="P567" t="inlineStr"/>
+      <c r="Q567" t="inlineStr"/>
+      <c r="R567" t="inlineStr"/>
+      <c r="S567" t="inlineStr"/>
+      <c r="T567" t="inlineStr"/>
+      <c r="U567" t="inlineStr"/>
+      <c r="V567" t="inlineStr"/>
+      <c r="W567" t="inlineStr"/>
+      <c r="X567" t="inlineStr"/>
+      <c r="Y567" t="inlineStr"/>
+      <c r="Z567" t="inlineStr"/>
+      <c r="AA567" t="inlineStr"/>
+      <c r="AB567" t="inlineStr"/>
+      <c r="AC567" t="inlineStr"/>
+      <c r="AD567" t="inlineStr"/>
+      <c r="AE567" t="inlineStr"/>
+      <c r="AF567" t="inlineStr"/>
+      <c r="AG567" t="inlineStr"/>
+      <c r="AH567" t="inlineStr"/>
+      <c r="AI567" t="inlineStr"/>
+      <c r="AJ567" t="inlineStr"/>
+      <c r="AK567" t="inlineStr"/>
+      <c r="AL567" t="inlineStr"/>
+      <c r="AM567" t="inlineStr"/>
+      <c r="AN567" t="inlineStr"/>
+      <c r="AO567" t="inlineStr"/>
+      <c r="AP567" t="inlineStr"/>
+      <c r="AQ567" t="inlineStr"/>
+      <c r="AR567" t="inlineStr"/>
+    </row>
+    <row r="568">
+      <c r="A568" s="1" t="n">
+        <v>566</v>
+      </c>
+      <c r="B568" t="inlineStr"/>
+      <c r="C568" t="inlineStr"/>
+      <c r="D568" t="inlineStr"/>
+      <c r="E568" t="inlineStr"/>
+      <c r="F568" t="inlineStr"/>
+      <c r="G568" t="inlineStr"/>
+      <c r="H568" t="inlineStr"/>
+      <c r="I568" t="inlineStr"/>
+      <c r="J568" t="inlineStr"/>
+      <c r="K568" t="inlineStr"/>
+      <c r="L568" t="inlineStr"/>
+      <c r="M568" t="inlineStr"/>
+      <c r="N568" t="inlineStr"/>
+      <c r="O568" t="inlineStr"/>
+      <c r="P568" t="inlineStr"/>
+      <c r="Q568" t="inlineStr"/>
+      <c r="R568" t="inlineStr"/>
+      <c r="S568" t="inlineStr"/>
+      <c r="T568" t="inlineStr"/>
+      <c r="U568" t="inlineStr"/>
+      <c r="V568" t="inlineStr"/>
+      <c r="W568" t="inlineStr"/>
+      <c r="X568" t="inlineStr"/>
+      <c r="Y568" t="inlineStr"/>
+      <c r="Z568" t="inlineStr"/>
+      <c r="AA568" t="inlineStr"/>
+      <c r="AB568" t="inlineStr"/>
+      <c r="AC568" t="inlineStr"/>
+      <c r="AD568" t="inlineStr"/>
+      <c r="AE568" t="inlineStr"/>
+      <c r="AF568" t="inlineStr"/>
+      <c r="AG568" t="inlineStr"/>
+      <c r="AH568" t="inlineStr"/>
+      <c r="AI568" t="inlineStr"/>
+      <c r="AJ568" t="inlineStr"/>
+      <c r="AK568" t="inlineStr"/>
+      <c r="AL568" t="inlineStr"/>
+      <c r="AM568" t="inlineStr"/>
+      <c r="AN568" t="inlineStr"/>
+      <c r="AO568" t="inlineStr"/>
+      <c r="AP568" t="inlineStr"/>
+      <c r="AQ568" t="inlineStr"/>
+      <c r="AR568" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>